<commit_message>
TAO LAO MIA LAO
CAP NHAT GIUM
</commit_message>
<xml_diff>
--- a/INFO.xlsx
+++ b/INFO.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="91">
   <si>
     <t>Shivapro123</t>
   </si>
@@ -286,6 +286,9 @@
   </si>
   <si>
     <t>pending</t>
+  </si>
+  <si>
+    <t>SHIVA GITHUB</t>
   </si>
 </sst>
 </file>
@@ -729,8 +732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:Y30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1073,6 +1076,9 @@
       </c>
     </row>
     <row r="22" spans="3:25" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
+        <v>90</v>
+      </c>
       <c r="M22" t="s">
         <v>41</v>
       </c>

</xml_diff>